<commit_message>
Update system CD, SD for Register user
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
@@ -183,17 +183,22 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8817376" cy="8058150"/>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>156708</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -206,8 +211,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="18964275"/>
-          <a:ext cx="8817376" cy="8058150"/>
+          <a:off x="0" y="762000"/>
+          <a:ext cx="9910308" cy="9105900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -215,7 +220,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -484,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update error lastname, firstname are require when validation
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Register user" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -489,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update API design for user login
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register user" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>REGISTER USER SEQUENCE DIAGRAM</t>
+  </si>
+  <si>
+    <t>LOGIN SEQUENCE DIAGRAM</t>
   </si>
 </sst>
 </file>
@@ -221,6 +225,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="10497964" cy="10039350"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123826" y="523875"/>
+          <a:ext cx="10497964" cy="10039350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -489,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1564,4 +1606,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit API design for User logout function
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Register user" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Logout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,12 +26,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>REGISTER USER SEQUENCE DIAGRAM</t>
   </si>
   <si>
     <t>LOGIN SEQUENCE DIAGRAM</t>
+  </si>
+  <si>
+    <t>LOGOUT SEQUENCE DIAGRAM</t>
   </si>
 </sst>
 </file>
@@ -263,6 +267,49 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>193810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="384310"/>
+          <a:ext cx="9963150" cy="5549765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1612,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,4 +1704,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update method PUT for user logout
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
@@ -275,19 +275,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>193810</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>404586</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -300,8 +300,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="384310"/>
-          <a:ext cx="9963150" cy="5549765"/>
+          <a:off x="485775" y="400050"/>
+          <a:ext cx="9062811" cy="5048250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1710,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update SD and Flow for update user info
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Register user" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Logout" sheetId="3" r:id="rId3"/>
+    <sheet name="Update user" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>REGISTER USER SEQUENCE DIAGRAM</t>
   </si>
@@ -35,6 +36,9 @@
   </si>
   <si>
     <t>LOGOUT SEQUENCE DIAGRAM</t>
+  </si>
+  <si>
+    <t>UPDATE USER SEQUENCE DIAGRAM</t>
   </si>
 </sst>
 </file>
@@ -302,6 +306,49 @@
         <a:xfrm>
           <a:off x="485775" y="400050"/>
           <a:ext cx="9062811" cy="5048250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>379454</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="495300"/>
+          <a:ext cx="10723604" cy="10001250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1710,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,4 +1802,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>